<commit_message>
[EGSVC-36] Added employee details folder
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/eisTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/eisTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="employeeDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,17 +22,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
   <si>
     <t xml:space="preserve">dataRow</t>
   </si>
   <si>
-    <t xml:space="preserve">EmployeeName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EmployeeCode</t>
-  </si>
-  <si>
     <t xml:space="preserve">EmployeeType</t>
   </si>
   <si>
@@ -54,7 +48,7 @@
     <t xml:space="preserve">IsUserActive</t>
   </si>
   <si>
-    <t xml:space="preserve">MobileNumber</t>
+    <t xml:space="preserve">Mobile</t>
   </si>
   <si>
     <t xml:space="preserve">PermanentAddress</t>
@@ -72,18 +66,15 @@
     <t xml:space="preserve">employee1</t>
   </si>
   <si>
-    <t xml:space="preserve">TestUser_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMP_01</t>
-  </si>
-  <si>
     <t xml:space="preserve">Permanent</t>
   </si>
   <si>
     <t xml:space="preserve">EMPLOYED</t>
   </si>
   <si>
+    <t xml:space="preserve">01/01/1990</t>
+  </si>
+  <si>
     <t xml:space="preserve">Male</t>
   </si>
   <si>
@@ -96,24 +87,30 @@
     <t xml:space="preserve">Yes</t>
   </si>
   <si>
-    <t xml:space="preserve">Municipal Office Rd, N.R.Peta, Near Appollo Hospital, Kurnool, Andhra Pradesh</t>
+    <t xml:space="preserve">9999999999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Municipal Office Rd, N.R.Peta, Near Appollo Hospital, Kurnool, Andhra Pradesh </t>
   </si>
   <si>
     <t xml:space="preserve">Kurnool</t>
   </si>
   <si>
+    <t xml:space="preserve">518004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/01/2012</t>
+  </si>
+  <si>
     <t xml:space="preserve">employee2</t>
   </si>
   <si>
-    <t xml:space="preserve">TestUser_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMP_02</t>
-  </si>
-  <si>
     <t xml:space="preserve">RETIRED</t>
   </si>
   <si>
+    <t xml:space="preserve">02/01/1990</t>
+  </si>
+  <si>
     <t xml:space="preserve">Female</t>
   </si>
   <si>
@@ -124,6 +121,12 @@
   </si>
   <si>
     <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8888888888</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/01/2012</t>
   </si>
   <si>
     <t xml:space="preserve">IsPrimary</t>
@@ -187,9 +190,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -256,8 +260,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -265,7 +273,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -286,31 +294,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1632653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.030612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.1938775510204"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.530612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.3673469387755"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0561224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0612244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.030612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.86224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.0612244897959"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.6683673469388"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.7551020408163"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.6122448979592"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.75"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.8877551020408"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
@@ -349,58 +358,46 @@
       <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="2" t="n">
-        <v>32874</v>
-      </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="K2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="0" t="n">
-        <v>9999999999</v>
-      </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="N2" s="0" t="n">
-        <v>518004</v>
-      </c>
-      <c r="O2" s="2" t="n">
-        <v>40909</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -408,52 +405,46 @@
         <v>26</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>18</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="2" t="n">
-        <v>32875</v>
+      <c r="F3" s="0" t="s">
+        <v>30</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="0" t="s">
         <v>32</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="J3" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>8888888888</v>
-      </c>
-      <c r="L3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" s="0" t="n">
-        <v>518004</v>
-      </c>
-      <c r="O3" s="2" t="n">
-        <v>40910</v>
+      <c r="M3" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -474,86 +465,86 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8877551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.0357142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.6479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="n">
         <v>40914</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="3" t="n">
         <v>41280</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="C3" s="3" t="n">
         <v>40915</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="3" t="n">
         <v>41281</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -568,15 +559,15 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="15.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.7040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -584,38 +575,38 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
[PHOENIX-5879] Modified the BillBasedReceipt according to production dump
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/eisTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/eisTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="employeeDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -156,7 +156,7 @@
     <t xml:space="preserve">ACCOUNTS</t>
   </si>
   <si>
-    <t xml:space="preserve">Accountant Category – IV</t>
+    <t xml:space="preserve">Accountant Category - IV</t>
   </si>
   <si>
     <t xml:space="preserve">ACC_Accountant_Category_1</t>
@@ -312,20 +312,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="1023" min="13" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="1023" min="13" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -445,7 +445,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -461,17 +461,17 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.7448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -520,7 +520,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
@@ -536,7 +536,7 @@
       <c r="E3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>44</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -546,7 +546,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -567,10 +567,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -609,7 +609,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
[EGSVC-36] Modified create employee feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/eisTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/eisTestData.xlsx
@@ -12,17 +12,17 @@
     <sheet name="assignmentDetails" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="jurisdictionList" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="71">
   <si>
     <t xml:space="preserve">dataRow</t>
   </si>
@@ -120,6 +120,33 @@
     <t xml:space="preserve">02/01/2012</t>
   </si>
   <si>
+    <t xml:space="preserve">employee3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deputation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DECEASED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7777777777</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/01/2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">employee4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outsourced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6666666666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/01/2014</t>
+  </si>
+  <si>
     <t xml:space="preserve">IsPrimary</t>
   </si>
   <si>
@@ -162,6 +189,21 @@
     <t xml:space="preserve">ACC_Accountant_Category_1</t>
   </si>
   <si>
+    <t xml:space="preserve">assignment3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accounts Officer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACC_ACC_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assignment4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACC_Accounts_Officer_001</t>
+  </si>
+  <si>
     <t xml:space="preserve">JurisdictionType</t>
   </si>
   <si>
@@ -181,6 +223,18 @@
   </si>
   <si>
     <t xml:space="preserve">Election Ward No. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JurisdictionList3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Election Ward No. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JurisdictionList4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Election Ward No. 3</t>
   </si>
 </sst>
 </file>
@@ -278,11 +332,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -304,28 +358,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="1023" min="13" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="66.4183673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1023" min="13" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -442,10 +495,80 @@
         <v>31</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>32143</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>33239</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -458,89 +581,134 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="4" t="n">
+      <c r="C2" s="5" t="n">
         <v>40914</v>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="D2" s="5" t="n">
         <v>41280</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="4" t="n">
+      <c r="C3" s="5" t="n">
         <v>42852</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="4" t="n">
         <v>42852</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>45</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>42860</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>42860</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>42891</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>42891</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -559,51 +727,73 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>52</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[PHOENIX-6078] UI : Added loop to insert the jurisdiction details in create employee feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/eisTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/eisTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="employeeDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -204,10 +204,10 @@
     <t xml:space="preserve">ACC_Accounts_Officer_001</t>
   </si>
   <si>
-    <t xml:space="preserve">JurisdictionType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JurisdictionList</t>
+    <t xml:space="preserve">jurisdictionType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jurisdictionList</t>
   </si>
   <si>
     <t xml:space="preserve">JurisdictionList1</t>
@@ -366,19 +366,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="66.4183673469388"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1023" min="13" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="65.6071428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="20.25"/>
+    <col collapsed="false" hidden="false" max="1023" min="13" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,7 +569,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -583,20 +584,20 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -714,7 +715,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -729,16 +730,17 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.7040816326531"/>
+    <col collapsed="false" hidden="false" max="1022" min="4" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -799,7 +801,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
[EGSVC-36] UI : Added the Position Data in employee excel and also made the position has auto selected
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/eisTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/eisTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="employeeDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
   <si>
     <t xml:space="preserve">dataRow</t>
   </si>
@@ -163,9 +163,6 @@
     <t xml:space="preserve">Designation</t>
   </si>
   <si>
-    <t xml:space="preserve">Position</t>
-  </si>
-  <si>
     <t xml:space="preserve">assignment1</t>
   </si>
   <si>
@@ -175,9 +172,6 @@
     <t xml:space="preserve">Assistant Engineer</t>
   </si>
   <si>
-    <t xml:space="preserve">ENG_Assistant Engineer_5</t>
-  </si>
-  <si>
     <t xml:space="preserve">assignment2</t>
   </si>
   <si>
@@ -187,22 +181,10 @@
     <t xml:space="preserve">Accountant Category - IV</t>
   </si>
   <si>
-    <t xml:space="preserve">ACC_Accountant_Category_1</t>
-  </si>
-  <si>
     <t xml:space="preserve">assignment3</t>
   </si>
   <si>
     <t xml:space="preserve">Accounts Officer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACC_ACC_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assignment4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACC_Accounts_Officer_001</t>
   </si>
   <si>
     <t xml:space="preserve">jurisdictionType</t>
@@ -381,20 +363,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="64.7959183673469"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="257" min="13" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="63.4438775510204"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="257" min="13" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -597,24 +579,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="254" min="6" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="255" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.3928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="254" min="6" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="255" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -627,73 +609,47 @@
       <c r="D1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -720,11 +676,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.1887755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,54 +688,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -800,23 +756,23 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -824,7 +780,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -832,7 +788,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -840,7 +796,7 @@
         <v>32</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>